<commit_message>
change the version of the Writing_to_diff.py
</commit_message>
<xml_diff>
--- a/Practice_problem/sheets.xlsx
+++ b/Practice_problem/sheets.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_Python\Practice_problem\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shivam\PycharmProjects\Python_Practice\Practice_problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="94">
   <si>
     <t>ID</t>
   </si>
@@ -303,11 +303,14 @@
   <si>
     <t>Data50</t>
   </si>
+  <si>
+    <t>rashma</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -662,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M45"/>
+  <dimension ref="A1:M46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,7 +760,7 @@
         <v>99003722</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -2513,6 +2516,17 @@
       </c>
       <c r="M45" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <v>99003734</v>
+      </c>
+      <c r="B46" t="s">
+        <v>93</v>
+      </c>
+      <c r="C46" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -2525,7 +2539,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M45"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
@@ -8106,10 +8120,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M65"/>
+  <dimension ref="A1:M66"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E46" sqref="E46"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10749,6 +10763,17 @@
         <v>45</v>
       </c>
     </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <v>99005050</v>
+      </c>
+      <c r="B66" t="s">
+        <v>44</v>
+      </c>
+      <c r="C66" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90"/>

</xml_diff>